<commit_message>
it's been a really long time lol
</commit_message>
<xml_diff>
--- a/Exercise/Laurel Workouts Possibly.xlsx
+++ b/Exercise/Laurel Workouts Possibly.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damir\OneDrive\Documents\UTK Spring '24\Exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EC74CA-6F4B-4448-B708-AA351DDF5827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7C0852-B2D6-4EF4-9ECE-05D20E212A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
   <si>
     <t>Previous Workouts</t>
   </si>
@@ -202,19 +213,124 @@
   </si>
   <si>
     <t>Incline Dumbbell Curl</t>
+  </si>
+  <si>
+    <t>Dumbells -5lb-60lb</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Triceps</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>Exercises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lats </t>
+  </si>
+  <si>
+    <t>Traps</t>
+  </si>
+  <si>
+    <t>Rhomboids</t>
+  </si>
+  <si>
+    <t>Biceps</t>
+  </si>
+  <si>
+    <t>Rear Delts</t>
+  </si>
+  <si>
+    <t>Forearms</t>
+  </si>
+  <si>
+    <t>Glutes</t>
+  </si>
+  <si>
+    <t>Quadriceps</t>
+  </si>
+  <si>
+    <t>Hamstrings</t>
+  </si>
+  <si>
+    <t>Calves</t>
+  </si>
+  <si>
+    <t>Abs</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>✓ (make sure to go deep)</t>
+  </si>
+  <si>
+    <t>Reps</t>
+  </si>
+  <si>
+    <t>5-12 per set, 'burnout' 20-30+</t>
+  </si>
+  <si>
+    <t>Dumbbell Upright Rows</t>
+  </si>
+  <si>
+    <t>✓ (non-elevated)</t>
+  </si>
+  <si>
+    <t>Split Squats/Bulgarian Split Squats</t>
+  </si>
+  <si>
+    <t>Dumbbell Romanian deadlifts</t>
+  </si>
+  <si>
+    <t>Standing One-Leg Calf Raise (Bodyweight or Dumbbell)</t>
+  </si>
+  <si>
+    <t>2 Second Hold On Top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overhead Two-Handed Rope Cable Extension </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Low Pulley</t>
+  </si>
+  <si>
+    <t>Cross-Body</t>
+  </si>
+  <si>
+    <t>Kneeling Cable Crunch</t>
+  </si>
+  <si>
+    <t>Reverse-Grip One-Arm Dumbbell Curls</t>
+  </si>
+  <si>
+    <t>Dumbell Lateral Raise</t>
+  </si>
+  <si>
+    <t>Dumbbel Frontal Raise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +341,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -371,11 +487,148 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -392,35 +645,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,48 +1051,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:L35"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B2:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="B32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
+    <col min="3" max="3" width="46.1796875" customWidth="1"/>
     <col min="4" max="4" width="24.90625" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.54296875" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="15.7265625" customWidth="1"/>
     <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="46" t="s">
         <v>42</v>
       </c>
     </row>
@@ -751,24 +1103,24 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="16"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="19"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="2" t="s">
         <v>56</v>
       </c>
@@ -781,11 +1133,11 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="6"/>
+      <c r="B5" s="44"/>
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="2" t="s">
         <v>43</v>
       </c>
@@ -798,11 +1150,11 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="6"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="19"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="2" t="s">
         <v>47</v>
       </c>
@@ -815,11 +1167,11 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="6"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="19"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
@@ -832,11 +1184,11 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="6"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="19"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
@@ -849,11 +1201,11 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="6"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="19"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
@@ -866,11 +1218,11 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
@@ -883,11 +1235,11 @@
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
+      <c r="B11" s="44"/>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="19"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
@@ -900,11 +1252,11 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="6"/>
+      <c r="B12" s="44"/>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
@@ -917,11 +1269,11 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="6"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="2" t="s">
         <v>43</v>
       </c>
@@ -934,11 +1286,11 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="6"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="9"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -951,11 +1303,11 @@
       <c r="L14" s="2"/>
     </row>
     <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="7"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
@@ -968,7 +1320,7 @@
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="43" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -987,8 +1339,8 @@
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="6"/>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1004,11 +1356,11 @@
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="9"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1021,8 +1373,8 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1038,8 +1390,8 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="44"/>
+      <c r="C20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -1055,11 +1407,11 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="44"/>
+      <c r="C21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="19"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="2" t="s">
         <v>43</v>
       </c>
@@ -1072,8 +1424,8 @@
       <c r="L21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="6"/>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="44"/>
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1089,11 +1441,11 @@
       <c r="L22" s="2"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="6"/>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="19"/>
+      <c r="D23" s="9"/>
       <c r="E23" s="2" t="s">
         <v>52</v>
       </c>
@@ -1106,11 +1458,11 @@
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="6"/>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="19"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="2" t="s">
         <v>58</v>
       </c>
@@ -1123,8 +1475,8 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="7"/>
-      <c r="C25" s="10" t="s">
+      <c r="B25" s="45"/>
+      <c r="C25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1140,13 +1492,13 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="43" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="19"/>
+      <c r="D26" s="9"/>
       <c r="E26" s="2" t="s">
         <v>43</v>
       </c>
@@ -1159,8 +1511,8 @@
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="6"/>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1176,8 +1528,8 @@
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="6"/>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -1193,11 +1545,11 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="6"/>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="19"/>
+      <c r="D29" s="9"/>
       <c r="E29" s="2" t="s">
         <v>54</v>
       </c>
@@ -1210,11 +1562,11 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="6"/>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="44"/>
+      <c r="C30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="19"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="2" t="s">
         <v>54</v>
       </c>
@@ -1227,8 +1579,8 @@
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="6"/>
-      <c r="C31" s="9" t="s">
+      <c r="B31" s="44"/>
+      <c r="C31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1244,11 +1596,11 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32" s="6"/>
-      <c r="C32" s="9" t="s">
+      <c r="B32" s="44"/>
+      <c r="C32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="19"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="2" t="s">
         <v>43</v>
       </c>
@@ -1261,8 +1613,8 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B33" s="6"/>
-      <c r="C33" s="9" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1278,11 +1630,11 @@
       <c r="L33" s="2"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="6"/>
-      <c r="C34" s="9" t="s">
+      <c r="B34" s="44"/>
+      <c r="C34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="19"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="2" t="s">
         <v>57</v>
       </c>
@@ -1295,11 +1647,11 @@
       <c r="L34" s="2"/>
     </row>
     <row r="35" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="7"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="45"/>
+      <c r="C35" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="19"/>
+      <c r="D35" s="9"/>
       <c r="E35" s="2" t="s">
         <v>55</v>
       </c>
@@ -1311,8 +1663,810 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
+    <row r="36" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E37" s="2"/>
+      <c r="F37" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I38" s="39"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B40" s="12"/>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B41" s="12"/>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B42" s="12"/>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B43" s="12"/>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="16"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B44" s="12"/>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B45" s="12"/>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B46" s="12"/>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B47" s="12"/>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B48" s="12"/>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="26"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B49" s="12"/>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B50" s="12"/>
+      <c r="C50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="16"/>
+      <c r="E50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="13"/>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="21"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="J52" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B53" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="16"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B54" s="12"/>
+      <c r="C54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="16"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B55" s="12"/>
+      <c r="C55" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="16"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B56" s="12"/>
+      <c r="C56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="16"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="26"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B57" s="12"/>
+      <c r="C57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="16"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B58" s="12"/>
+      <c r="C58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J58" s="2"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B59" s="12"/>
+      <c r="C59" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B60" s="12"/>
+      <c r="C60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H60" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B61" s="6"/>
+      <c r="C61" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J61" s="2"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B62" s="6"/>
+      <c r="C62" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B63" s="6"/>
+      <c r="C63" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K63" s="33"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B64" s="6"/>
+      <c r="C64" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="16"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K64" s="33"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="7"/>
+      <c r="C65" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="16"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="27"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J66" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="K66" s="19"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B67" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="26"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B68" s="6"/>
+      <c r="C68" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="26"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B69" s="6"/>
+      <c r="C69" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="16"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="26"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B70" s="6"/>
+      <c r="C70" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="26"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B71" s="6"/>
+      <c r="C71" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="26"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B72" s="6"/>
+      <c r="C72" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="26"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B73" s="6"/>
+      <c r="C73" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="26"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B74" s="6"/>
+      <c r="C74" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="16"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B75" s="6"/>
+      <c r="C75" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G75" s="2"/>
+      <c r="H75" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="26"/>
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="7"/>
+      <c r="C76" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="26"/>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+      <c r="C77" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="15"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G77" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="26"/>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+      <c r="C78" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" s="16"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="26"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+      <c r="C79" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D79" s="38"/>
+      <c r="E79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J79" s="2"/>
+      <c r="K79" s="26"/>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+      <c r="C80" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="17"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="34"/>
+      <c r="J80" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="K80" s="23"/>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="B4:B15"/>
+    <mergeCell ref="B16:B25"/>
+    <mergeCell ref="B26:B35"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="J2:J3"/>
@@ -1322,9 +2476,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B4:B15"/>
-    <mergeCell ref="B16:B25"/>
-    <mergeCell ref="B26:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>